<commit_message>
Add main application window and configuration modules
Introduced `main_window.py` for GUI and worker logic, and `config.py` for reusable constants. Includes logging setup, UI logging integration, and enhancements for thread processing with PyQt.
</commit_message>
<xml_diff>
--- a/dati.xlsx
+++ b/dati.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4110" yWindow="1815" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -160,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -240,6 +240,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,32 +750,32 @@
           <t>1743573696146</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="28" t="inlineStr">
         <is>
           <t>1743573696146</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-942109</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -787,32 +790,32 @@
           <t>1743668858768</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="28" t="inlineStr">
         <is>
           <t>1743668858768</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-941686</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" s="28" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="17" t="n">
@@ -823,32 +826,32 @@
           <t>1744015060675</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="F4" s="28" t="inlineStr">
         <is>
           <t>1744015060675</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-942254</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -863,32 +866,32 @@
           <t>1744019120533</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="F5" s="28" t="inlineStr">
         <is>
           <t>1744019120533</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-941902</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -903,32 +906,32 @@
           <t>1744011702763</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="28" t="inlineStr">
         <is>
           <t>NON AMMISSIONE</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F6" s="3" t="inlineStr">
+      <c r="F6" s="28" t="inlineStr">
         <is>
           <t>1744011702763</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-941743</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -943,32 +946,32 @@
           <t>1744109260306</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F7" s="28" t="inlineStr">
         <is>
           <t>1744109260306</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-942164</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -983,32 +986,32 @@
           <t>1744199103851</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="F8" s="28" t="inlineStr">
         <is>
           <t>1744199103851</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-941732</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1023,32 +1026,32 @@
           <t>1744190924214</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F9" s="3" t="inlineStr">
+      <c r="F9" s="28" t="inlineStr">
         <is>
           <t>1744190924214</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-942157</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1063,32 +1066,32 @@
           <t>1744191503522</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F10" s="3" t="inlineStr">
+      <c r="F10" s="28" t="inlineStr">
         <is>
           <t>1744191503522</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G10" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-942160</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H10" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1103,32 +1106,32 @@
           <t>1744194879147</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="28" t="inlineStr">
         <is>
           <t>18/04/2025</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="F11" s="28" t="inlineStr">
         <is>
           <t>1744194879147</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-941985</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H11" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1143,32 +1146,32 @@
           <t>1744198815465</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="28" t="inlineStr">
         <is>
           <t>CHIUSA</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="28" t="inlineStr">
         <is>
           <t>RILASCIO NULLA OSTA</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="28" t="inlineStr">
         <is>
           <t>15/04/2025</t>
         </is>
       </c>
-      <c r="F12" s="3" t="inlineStr">
+      <c r="F12" s="28" t="inlineStr">
         <is>
           <t>1744198815465</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" s="28" t="inlineStr">
         <is>
           <t>2025-USMAF-MIL-GME-P-MXP-940160</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H12" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1181,32 +1184,32 @@
           <t>1744203024278</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="28" t="inlineStr">
         <is>
           <t>IN LAVORAZIONE</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F13" s="3" t="inlineStr">
+      <c r="F13" s="28" t="inlineStr">
         <is>
           <t>1744203024278</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="H13" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1221,32 +1224,32 @@
           <t>1744280580696</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="28" t="inlineStr">
         <is>
           <t>IN LAVORAZIONE</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F14" s="3" t="inlineStr">
+      <c r="F14" s="28" t="inlineStr">
         <is>
           <t>1744280580696</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" s="28" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="13" t="n">
@@ -1257,32 +1260,32 @@
           <t>1744350901846</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="28" t="inlineStr">
         <is>
           <t>IN LAVORAZIONE</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F15" s="3" t="inlineStr">
+      <c r="F15" s="28" t="inlineStr">
         <is>
           <t>1744350901846</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H15" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
UI Enhancement: Elegant file selection design with glassmorphism effects
- Redesigned file selection area with elegant container
- Added smooth animations for file display
- Implemented success indicators with pulse effects
- Fixed button transformation issues
- Added debug logging for troubleshooting
- Improved overall visual consistency
- Enhanced user experience with modern design patterns
</commit_message>
<xml_diff>
--- a/dati.xlsx
+++ b/dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stosello\nsis\ControlloStatoNSIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itose\cursor project\ControlloStatoNSIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3B8505-129F-4408-A993-F1001DF08DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEA5AAC-71E2-4854-ACA2-B78651A05CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="3480" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="2160" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>AWB</t>
   </si>
@@ -49,112 +49,43 @@
     <t>1743573696146</t>
   </si>
   <si>
-    <t>CHIUSA</t>
-  </si>
-  <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-942109</t>
-  </si>
-  <si>
-    <t>RILASCIO NULLA OSTA</t>
-  </si>
-  <si>
-    <t>18/04/2025</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>1743668858768</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-941686</t>
-  </si>
-  <si>
     <t>1744015060675</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-942254</t>
-  </si>
-  <si>
     <t>1744019120533</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-941902</t>
-  </si>
-  <si>
     <t>1744011702763</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-941743</t>
-  </si>
-  <si>
-    <t>NON AMMISSIONE</t>
-  </si>
-  <si>
     <t>1744109260306</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-942164</t>
-  </si>
-  <si>
     <t>1744199103851</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-941732</t>
-  </si>
-  <si>
     <t>1744190924214</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-942157</t>
-  </si>
-  <si>
     <t>1744191503522</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-942160</t>
-  </si>
-  <si>
     <t>1744194879147</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-941985</t>
-  </si>
-  <si>
     <t>1744198815465</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-940160</t>
-  </si>
-  <si>
-    <t>15/04/2025</t>
-  </si>
-  <si>
     <t>1744203024278</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-943382</t>
-  </si>
-  <si>
-    <t>23/04/2025</t>
-  </si>
-  <si>
     <t>1744280580696</t>
   </si>
   <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-942507</t>
-  </si>
-  <si>
-    <t>22/04/2025</t>
-  </si>
-  <si>
     <t>1744350901846</t>
-  </si>
-  <si>
-    <t>2025-USMAF-MIL-GME-P-MXP-944140</t>
-  </si>
-  <si>
-    <t>24/04/2025</t>
   </si>
 </sst>
 </file>
@@ -700,7 +631,7 @@
   <dimension ref="A1:H243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="C2:H4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,47 +679,25 @@
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>13</v>
-      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>8409370292</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>14</v>
-      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -796,281 +705,151 @@
         <v>2514430365</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>4104826961</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>1406381605</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>13</v>
-      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>4730077881</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="29" t="s">
         <v>13</v>
       </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>3649213724</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>5057815265</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="29" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>5057815276</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>7402858492</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="29" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>1562375592</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>13</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>8709762762</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>39</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1078,26 +857,14 @@
         <v>5559289455</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="29" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>

</xml_diff>